<commit_message>
feat(instances): national nandu 2024
</commit_message>
<xml_diff>
--- a/public/files/nacional/nandu/PedidoFactura.xlsx
+++ b/public/files/nacional/nandu/PedidoFactura.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marit\Dropbox\Ñandú\2023\competencias_ñandu\Nacional\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marit\Dropbox\Ñandú\2024\Competencias_nandu\Nacional\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5DE53A3-3C96-46D1-8FDB-1130C4CCE5C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7D8F7FD1-DA51-4130-ACC1-2794BB26BC5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,14 +18,14 @@
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Hoja1!$A$1:$G$9</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Hoja1!$A$1:$J$9</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Nombre</t>
   </si>
@@ -82,22 +82,51 @@
     </r>
   </si>
   <si>
-    <t>Concepto a facturar****</t>
-  </si>
-  <si>
     <t>Si es depósito, transferencia o efectivo.**</t>
   </si>
   <si>
     <t xml:space="preserve">**ADJUNTAR DEPOSITO/TRANSFERENCIA </t>
   </si>
   <si>
-    <t>Aclarar dirección*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">*hay instituciones que poseen más de una dirección </t>
-  </si>
-  <si>
-    <t xml:space="preserve">**** Discriminar cantidad de alojados,  alumnos sin alojamiento, acompañantes sin alojamiento y tarjeta (cada ítem tiene un valor diferente)   </t>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">(dirección postal si tuviera más de una)  </t>
+    </r>
+  </si>
+  <si>
+    <t>Alojados</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alumnos sin aloj. </t>
+  </si>
+  <si>
+    <t>Acompañantes sin aloj.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">**** Discriminar cantidad y competencia  </t>
+  </si>
+  <si>
+    <t>Concepto a facturar - CANTIDADES ****</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tarjeta Premiación </t>
   </si>
 </sst>
 </file>
@@ -107,7 +136,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -147,23 +176,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <i/>
-      <sz val="16"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -179,7 +191,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -215,11 +227,74 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -233,16 +308,34 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -552,10 +645,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -565,94 +658,125 @@
     <col min="3" max="3" width="24.44140625" style="1" customWidth="1"/>
     <col min="4" max="4" width="37" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26.88671875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="22.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="41" style="1" customWidth="1"/>
-    <col min="8" max="8" width="38.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="11.44140625" style="1"/>
+    <col min="6" max="6" width="18" style="1" customWidth="1"/>
+    <col min="7" max="7" width="18.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23" style="1" customWidth="1"/>
+    <col min="9" max="9" width="18.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="38.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="11.44140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" customFormat="1" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:11" customFormat="1" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="24.9" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="13"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>6</v>
-      </c>
+      <c r="G2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" s="7"/>
+      <c r="K2" s="9"/>
     </row>
-    <row r="2" spans="1:8" ht="24.9" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-    </row>
-    <row r="3" spans="1:8" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="24.9" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="3"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
     </row>
-    <row r="4" spans="1:8" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="3"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
     </row>
-    <row r="5" spans="1:8" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="F5" s="3"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
     </row>
-    <row r="7" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="7" t="s">
-        <v>10</v>
+    <row r="7" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="6" t="s">
-        <v>9</v>
+    <row r="8" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="K1:K2"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+  </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.31496062992125984" right="0.31496062992125984" top="0.74803149606299213" bottom="0.55118110236220474" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="5" scale="98" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>